<commit_message>
VISBO SPE: changed the window for the settings; new function add/delete ressources with right click on the column projectName or variantName or businessUnit or phaseName
</commit_message>
<xml_diff>
--- a/VISBO SPE/VSIBO SPE/VISBO Project Edit.xlsx
+++ b/VISBO SPE/VSIBO SPE/VISBO Project Edit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UteRittinghaus-Koyte\Dokumente\VISBO-NativeClients\visbo-projectboard\VISBO SPE\VSIBO SPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED94C128-D138-42C5-99D9-3AC8EDC48D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7611F6-DEA1-4821-9B7B-9908A172740F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D60B5602-748C-446A-ABEB-E0E5256C4A6F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D60B5602-748C-446A-ABEB-E0E5256C4A6F}"/>
   </bookViews>
   <sheets>
     <sheet name="meTE" sheetId="3" r:id="rId1"/>
@@ -74,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -404,15 +405,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1B2A9A-0267-4B2F-B27C-A850DCF35502}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="11.42578125" style="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -421,7 +426,7 @@
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
VISBO SPE: no marked cells, next version
</commit_message>
<xml_diff>
--- a/VISBO SPE/VSIBO SPE/VISBO Project Edit.xlsx
+++ b/VISBO SPE/VSIBO SPE/VISBO Project Edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UteRittinghaus-Koyte\Dokumente\VISBO-NativeClients\visbo-projectboard\VISBO SPE\VSIBO SPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7611F6-DEA1-4821-9B7B-9908A172740F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02FE72F-BADD-4C56-BCA0-6EE78276A031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D60B5602-748C-446A-ABEB-E0E5256C4A6F}"/>
   </bookViews>
@@ -407,9 +407,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>